<commit_message>
added kfb slide cutting support IMPORTANT
</commit_message>
<xml_diff>
--- a/res/标记数据分配.xlsx
+++ b/res/标记数据分配.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202">
   <si>
     <t>人员</t>
   </si>
@@ -612,6 +612,15 @@
   </si>
   <si>
     <t>2018-06-01_12_45_07</t>
+  </si>
+  <si>
+    <t>2018-06-01_12_47_17</t>
+  </si>
+  <si>
+    <t>2018-06-01_12_50_09</t>
+  </si>
+  <si>
+    <t>2018-06-01_12_54_50</t>
   </si>
 </sst>
 </file>
@@ -621,8 +630,8 @@
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ \￥* #,##0_ ;_ \￥* \-#,##0_ ;_ \￥* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ \￥* #,##0.00_ ;_ \￥* \-#,##0.00_ ;_ \￥* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ \￥* #,##0.00_ ;_ \￥* \-#,##0.00_ ;_ \￥* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ \￥* #,##0_ ;_ \￥* \-#,##0_ ;_ \￥* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -658,7 +667,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -667,14 +675,21 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -690,9 +705,41 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -712,40 +759,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -759,8 +774,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -782,14 +798,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -804,7 +813,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -816,175 +993,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1000,29 +1009,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1057,6 +1046,24 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -1068,6 +1075,17 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1086,19 +1104,10 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1107,139 +1116,139 @@
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2349,10 +2358,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:U83"/>
+  <dimension ref="A1:U86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="C83" sqref="C83"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="C86" sqref="C86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
@@ -3680,6 +3689,33 @@
         <v>198</v>
       </c>
     </row>
+    <row r="84" spans="1:3">
+      <c r="A84" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="85" spans="2:3">
+      <c r="B85" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="86" spans="2:3">
+      <c r="B86" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>201</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="A12:A13"/>

</xml_diff>